<commit_message>
Updated Excel file with searching workbook for domains that have other or 0 as their values
</commit_message>
<xml_diff>
--- a/processed_new_data.xlsx
+++ b/processed_new_data.xlsx
@@ -8,15 +8,29 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kristjan\Desktop\idsproj\listings\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{2081DD57-FF46-4E8D-BCF5-0BA05734078C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABDA4BF5-EDAF-4329-8CAD-DDFE51EB5638}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21270" windowHeight="15600" activeTab="1" xr2:uid="{9CA2BB68-6A21-43A2-9FF7-FEF8DF179EC9}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16950" windowHeight="15600" firstSheet="1" activeTab="2" xr2:uid="{9CA2BB68-6A21-43A2-9FF7-FEF8DF179EC9}"/>
   </bookViews>
   <sheets>
     <sheet name="processed_new_data" sheetId="1" r:id="rId1"/>
     <sheet name="FilteredRowsByDomain" sheetId="2" r:id="rId2"/>
+    <sheet name="SearchInOtherOrZeroDomain" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -43,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8488" uniqueCount="3630">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8497" uniqueCount="3633">
   <si>
     <t>company_name</t>
   </si>
@@ -10933,6 +10947,15 @@
   </si>
   <si>
     <t>Unique domains for reference</t>
+  </si>
+  <si>
+    <t>Search for keywords in job_name in domains with other or 0 value</t>
+  </si>
+  <si>
+    <t>Searchword (case insensitive):</t>
+  </si>
+  <si>
+    <t>senior</t>
   </si>
 </sst>
 </file>
@@ -11075,7 +11098,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -11255,6 +11278,12 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.749992370372631"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -11416,12 +11445,13 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="fill"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -54290,8 +54320,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47998272-36F4-4D82-97E3-A95B365160B6}">
   <dimension ref="A1:K515"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView topLeftCell="A124" zoomScale="120" workbookViewId="0">
+      <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -64687,4 +64717,1216 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B89310B-343D-4C0D-B2AF-71E8ECF3DFDF}">
+  <dimension ref="A1:G59"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="58.42578125" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" customWidth="1"/>
+    <col min="3" max="3" width="61" customWidth="1"/>
+    <col min="5" max="5" width="20.42578125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="41.42578125" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>3630</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3631</v>
+      </c>
+      <c r="B2" t="str" cm="1">
+        <f t="array" ref="B2:G59">_xlfn._xlws.SORT(_xlfn._xlws.FILTER(FilteredRowsByDomain!A2:F2129, ISNUMBER(SEARCH(A3, FilteredRowsByDomain!B2:B2129))), 2, 1)</f>
+        <v>wise</v>
+      </c>
+      <c r="C2" t="str">
+        <v>cdd quality senior specialist - maternity leave cover</v>
+      </c>
+      <c r="D2" t="str">
+        <v>other</v>
+      </c>
+      <c r="E2" s="1">
+        <v>45425</v>
+      </c>
+      <c r="F2" s="1">
+        <v>45425</v>
+      </c>
+      <c r="G2" t="str">
+        <v>https://jobs.smartrecruiters.com/wise/743999987082533</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>3632</v>
+      </c>
+      <c r="B3" t="str">
+        <v>wise</v>
+      </c>
+      <c r="C3" t="str">
+        <v>compliance senior specialist</v>
+      </c>
+      <c r="D3" t="str">
+        <v>other</v>
+      </c>
+      <c r="E3" s="1">
+        <v>45561</v>
+      </c>
+      <c r="F3" s="1">
+        <v>45586</v>
+      </c>
+      <c r="G3" t="str">
+        <v>https://jobs.smartrecruiters.com/wise/744000016541009</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B4" t="str">
+        <v>wise</v>
+      </c>
+      <c r="C4" t="str">
+        <v>display senior executive</v>
+      </c>
+      <c r="D4" t="str">
+        <v>other</v>
+      </c>
+      <c r="E4" s="1">
+        <v>45570</v>
+      </c>
+      <c r="F4" s="1">
+        <v>45576</v>
+      </c>
+      <c r="G4" t="str">
+        <v>https://jobs.smartrecruiters.com/wise/744000018604752</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B5" t="str">
+        <v>wise</v>
+      </c>
+      <c r="C5" t="str">
+        <v>display senior executive</v>
+      </c>
+      <c r="D5" t="str">
+        <v>other</v>
+      </c>
+      <c r="E5" s="1">
+        <v>45577</v>
+      </c>
+      <c r="F5" s="1">
+        <v>45578</v>
+      </c>
+      <c r="G5" t="str">
+        <v>https://jobs.smartrecruiters.com/wise/744000019891378</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B6" t="str">
+        <v>wise</v>
+      </c>
+      <c r="C6" t="str">
+        <v>display senior executive</v>
+      </c>
+      <c r="D6" t="str">
+        <v>other</v>
+      </c>
+      <c r="E6" s="1">
+        <v>45579</v>
+      </c>
+      <c r="F6" s="1">
+        <v>45579</v>
+      </c>
+      <c r="G6" t="str">
+        <v>https://jobs.smartrecruiters.com/wise/744000020190375</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B7" t="str">
+        <v>wise</v>
+      </c>
+      <c r="C7" t="str">
+        <v>display senior executive</v>
+      </c>
+      <c r="D7" t="str">
+        <v>other</v>
+      </c>
+      <c r="E7" s="1">
+        <v>45580</v>
+      </c>
+      <c r="F7" s="1">
+        <v>45580</v>
+      </c>
+      <c r="G7" t="str">
+        <v>https://jobs.smartrecruiters.com/wise/744000020400936</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B8" t="str">
+        <v>wise</v>
+      </c>
+      <c r="C8" t="str">
+        <v>global regulatory compliance senior specialist</v>
+      </c>
+      <c r="D8" t="str">
+        <v>other</v>
+      </c>
+      <c r="E8" s="1">
+        <v>45399</v>
+      </c>
+      <c r="F8" s="1">
+        <v>45426</v>
+      </c>
+      <c r="G8" t="str">
+        <v>https://jobs.smartrecruiters.com/wise/743999980555673</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B9" t="str">
+        <v>wise</v>
+      </c>
+      <c r="C9" t="str">
+        <v>programmatic senior executive</v>
+      </c>
+      <c r="D9" t="str">
+        <v>other</v>
+      </c>
+      <c r="E9" s="1">
+        <v>45581</v>
+      </c>
+      <c r="F9" s="1">
+        <v>45606</v>
+      </c>
+      <c r="G9" t="str">
+        <v>https://jobs.smartrecruiters.com/wise/744000020706181</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B10" t="str">
+        <v>luminor</v>
+      </c>
+      <c r="C10" t="str">
+        <v>regulatory inspections senior officer</v>
+      </c>
+      <c r="D10" t="str">
+        <v>other</v>
+      </c>
+      <c r="E10" s="1">
+        <v>45492</v>
+      </c>
+      <c r="F10" s="1">
+        <v>45495</v>
+      </c>
+      <c r="G10" t="str">
+        <v>https://luminorbank.teamtailor.com/jobs/4756550-regulatory-inspections-senior-officer</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B11" t="str">
+        <v>wolt</v>
+      </c>
+      <c r="C11" t="str">
+        <v>senior accounts receivable specialist</v>
+      </c>
+      <c r="D11" t="str">
+        <v>other</v>
+      </c>
+      <c r="E11" s="1">
+        <v>45576</v>
+      </c>
+      <c r="F11" s="1">
+        <v>45593</v>
+      </c>
+      <c r="G11" t="str">
+        <v>https://jobs.smartrecruiters.com/wolt/744000019838355</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B12" t="str">
+        <v>luminor</v>
+      </c>
+      <c r="C12" t="str">
+        <v>senior anti-fraud compliance officer</v>
+      </c>
+      <c r="D12" t="str">
+        <v>other</v>
+      </c>
+      <c r="E12" s="1">
+        <v>45601</v>
+      </c>
+      <c r="F12" s="1">
+        <v>45606</v>
+      </c>
+      <c r="G12" t="str">
+        <v>https://luminorbank.teamtailor.com/jobs/5157778-senior-anti-fraud-compliance-officer</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B13" t="str">
+        <v>bolt</v>
+      </c>
+      <c r="C13" t="str">
+        <v>senior benefits specialist</v>
+      </c>
+      <c r="D13" t="str">
+        <v>other</v>
+      </c>
+      <c r="E13" s="1">
+        <v>45602</v>
+      </c>
+      <c r="F13" s="1">
+        <v>45606</v>
+      </c>
+      <c r="G13" t="str">
+        <v>https://careers.bolt.eu/positions/7717376002</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B14" t="str">
+        <v>bolt</v>
+      </c>
+      <c r="C14" t="str">
+        <v>senior bid writer</v>
+      </c>
+      <c r="D14" t="str">
+        <v>other</v>
+      </c>
+      <c r="E14" s="1">
+        <v>45449</v>
+      </c>
+      <c r="F14" s="1">
+        <v>45499</v>
+      </c>
+      <c r="G14" t="str">
+        <v>https://careers.bolt.eu/positions/7456560002</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B15" t="str">
+        <v>bolt</v>
+      </c>
+      <c r="C15" t="str">
+        <v>senior bid writer</v>
+      </c>
+      <c r="D15" t="str">
+        <v>other</v>
+      </c>
+      <c r="E15" s="1">
+        <v>45458</v>
+      </c>
+      <c r="F15" s="1">
+        <v>45502</v>
+      </c>
+      <c r="G15" t="str">
+        <v>https://careers.bolt.eu/positions/7465401002</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B16" t="str">
+        <v>bolt</v>
+      </c>
+      <c r="C16" t="str">
+        <v>senior bid writer</v>
+      </c>
+      <c r="D16" t="str">
+        <v>other</v>
+      </c>
+      <c r="E16" s="1">
+        <v>45448</v>
+      </c>
+      <c r="F16" s="1">
+        <v>45493</v>
+      </c>
+      <c r="G16" t="str">
+        <v>https://careers.bolt.eu/positions/7465402002</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B17" t="str">
+        <v>bolt</v>
+      </c>
+      <c r="C17" t="str">
+        <v>senior bid writer</v>
+      </c>
+      <c r="D17" t="str">
+        <v>other</v>
+      </c>
+      <c r="E17" s="1">
+        <v>45446</v>
+      </c>
+      <c r="F17" s="1">
+        <v>45501</v>
+      </c>
+      <c r="G17" t="str">
+        <v>https://careers.bolt.eu/positions/7465410002</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B18" t="str">
+        <v>bolt</v>
+      </c>
+      <c r="C18" t="str">
+        <v>senior bid writer</v>
+      </c>
+      <c r="D18" t="str">
+        <v>other</v>
+      </c>
+      <c r="E18" s="1">
+        <v>45455</v>
+      </c>
+      <c r="F18" s="1">
+        <v>45492</v>
+      </c>
+      <c r="G18" t="str">
+        <v>https://careers.bolt.eu/positions/7465472002</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B19" t="str">
+        <v>pipedrive</v>
+      </c>
+      <c r="C19" t="str">
+        <v>senior brand manager</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19" s="1">
+        <v>45377</v>
+      </c>
+      <c r="F19" s="1">
+        <v>45377</v>
+      </c>
+      <c r="G19" t="str">
+        <v>https://jobs.lever.co/pipedrive/bd1b0b9f-f3fe-4731-b079-70c031d430e9</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B20" t="str">
+        <v>veriff</v>
+      </c>
+      <c r="C20" t="str">
+        <v>senior commercial counsel (emea)</v>
+      </c>
+      <c r="D20" t="str">
+        <v>other</v>
+      </c>
+      <c r="E20" s="1">
+        <v>45377</v>
+      </c>
+      <c r="F20" s="1">
+        <v>45386</v>
+      </c>
+      <c r="G20" t="str">
+        <v>https://www.veriff.com/careers/position/7278054002?gh_jid=7278054002</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B21" t="str">
+        <v>luminor</v>
+      </c>
+      <c r="C21" t="str">
+        <v>senior compliance officer (assurance unit)</v>
+      </c>
+      <c r="D21" t="str">
+        <v>other</v>
+      </c>
+      <c r="E21" s="1">
+        <v>45384</v>
+      </c>
+      <c r="F21" s="1">
+        <v>45578</v>
+      </c>
+      <c r="G21" t="str">
+        <v>https://luminorbank.teamtailor.com/jobs/3541206-senior-compliance-officer-assurance-unit</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B22" t="str">
+        <v>luminor</v>
+      </c>
+      <c r="C22" t="str">
+        <v>senior compliance officer (conduct)</v>
+      </c>
+      <c r="D22" t="str">
+        <v>other</v>
+      </c>
+      <c r="E22" s="1">
+        <v>45502</v>
+      </c>
+      <c r="F22" s="1">
+        <v>45516</v>
+      </c>
+      <c r="G22" t="str">
+        <v>https://luminorbank.teamtailor.com/jobs/4760679-senior-compliance-officer-conduct</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B23" t="str">
+        <v>luminor</v>
+      </c>
+      <c r="C23" t="str">
+        <v>senior compliance officer (conduct)</v>
+      </c>
+      <c r="D23" t="str">
+        <v>other</v>
+      </c>
+      <c r="E23" s="1">
+        <v>45593</v>
+      </c>
+      <c r="F23" s="1">
+        <v>45606</v>
+      </c>
+      <c r="G23" t="str">
+        <v>https://luminorbank.teamtailor.com/jobs/5133466-senior-compliance-officer-conduct</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B24" t="str">
+        <v>luminor</v>
+      </c>
+      <c r="C24" t="str">
+        <v>senior compliance officer (investment services)</v>
+      </c>
+      <c r="D24" t="str">
+        <v>other</v>
+      </c>
+      <c r="E24" s="1">
+        <v>45411</v>
+      </c>
+      <c r="F24" s="1">
+        <v>45424</v>
+      </c>
+      <c r="G24" t="str">
+        <v>https://luminorbank.teamtailor.com/jobs/4111511-senior-compliance-officer-investment-services</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B25" t="str">
+        <v>luminor</v>
+      </c>
+      <c r="C25" t="str">
+        <v>senior compliance officer (risk analysis &amp; reporting unit)</v>
+      </c>
+      <c r="D25" t="str">
+        <v>other</v>
+      </c>
+      <c r="E25" s="1">
+        <v>45377</v>
+      </c>
+      <c r="F25" s="1">
+        <v>45478</v>
+      </c>
+      <c r="G25" t="str">
+        <v>https://luminorbank.teamtailor.com/jobs/3712869-senior-compliance-officer-risk-analysis-reporting-unit</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B26" t="str">
+        <v>luminor</v>
+      </c>
+      <c r="C26" t="str">
+        <v>senior compliance officer (sanctions compliance)</v>
+      </c>
+      <c r="D26" t="str">
+        <v>other</v>
+      </c>
+      <c r="E26" s="1">
+        <v>45568</v>
+      </c>
+      <c r="F26" s="1">
+        <v>45585</v>
+      </c>
+      <c r="G26" t="str">
+        <v>https://luminorbank.teamtailor.com/jobs/5043485-senior-compliance-officer-sanctions-compliance</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B27" t="str">
+        <v>luminor</v>
+      </c>
+      <c r="C27" t="str">
+        <v>senior compliance officer (sanctions governance&amp;advisory)</v>
+      </c>
+      <c r="D27" t="str">
+        <v>other</v>
+      </c>
+      <c r="E27" s="1">
+        <v>45440</v>
+      </c>
+      <c r="F27" s="1">
+        <v>45552</v>
+      </c>
+      <c r="G27" t="str">
+        <v>https://luminorbank.teamtailor.com/jobs/3510229-senior-compliance-officer-sanctions-governance-advisory</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B28" t="str">
+        <v>bolt</v>
+      </c>
+      <c r="C28" t="str">
+        <v>senior consolidation specialist</v>
+      </c>
+      <c r="D28" t="str">
+        <v>other</v>
+      </c>
+      <c r="E28" s="1">
+        <v>45377</v>
+      </c>
+      <c r="F28" s="1">
+        <v>45387</v>
+      </c>
+      <c r="G28" t="str">
+        <v>https://careers.bolt.eu/positions/7256972002</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B29" t="str">
+        <v>swedbank</v>
+      </c>
+      <c r="C29" t="str">
+        <v>senior credit risk modeller</v>
+      </c>
+      <c r="D29" t="str">
+        <v>other</v>
+      </c>
+      <c r="E29" s="1">
+        <v>45377</v>
+      </c>
+      <c r="F29" s="1">
+        <v>45391</v>
+      </c>
+      <c r="G29" t="str">
+        <v>https://jobs.swedbank.com/jobs/18346-senior-credit-risk-modeller</v>
+      </c>
+    </row>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B30" t="str">
+        <v>swedbank</v>
+      </c>
+      <c r="C30" t="str">
+        <v>senior credit risk modeller</v>
+      </c>
+      <c r="D30" t="str">
+        <v>other</v>
+      </c>
+      <c r="E30" s="1">
+        <v>45430</v>
+      </c>
+      <c r="F30" s="1">
+        <v>45529</v>
+      </c>
+      <c r="G30" t="str">
+        <v>https://jobs.swedbank.com/jobs/18948-senior-credit-risk-modeller</v>
+      </c>
+    </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B31" t="str">
+        <v>bolt</v>
+      </c>
+      <c r="C31" t="str">
+        <v>senior data analyst, applied marketing measurements</v>
+      </c>
+      <c r="D31">
+        <v>0</v>
+      </c>
+      <c r="E31" s="1">
+        <v>45377</v>
+      </c>
+      <c r="F31" s="1">
+        <v>45377</v>
+      </c>
+      <c r="G31" t="str">
+        <v>https://careers.bolt.eu/positions/7298651002</v>
+      </c>
+    </row>
+    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B32" t="str">
+        <v>bally's interactive</v>
+      </c>
+      <c r="C32" t="str">
+        <v>senior data engineer</v>
+      </c>
+      <c r="D32">
+        <v>0</v>
+      </c>
+      <c r="E32" s="1">
+        <v>45377</v>
+      </c>
+      <c r="F32" s="1">
+        <v>45377</v>
+      </c>
+      <c r="G32" t="str">
+        <v>https://careers.ballysinteractive.com/jobs?id=5825791&amp;gh_jid=5825791</v>
+      </c>
+    </row>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B33" t="str">
+        <v>wolt</v>
+      </c>
+      <c r="C33" t="str">
+        <v>senior flutter engineer, in-store and merchant operations</v>
+      </c>
+      <c r="D33" t="str">
+        <v>other</v>
+      </c>
+      <c r="E33" s="1">
+        <v>45582</v>
+      </c>
+      <c r="F33" s="1">
+        <v>45596</v>
+      </c>
+      <c r="G33" t="str">
+        <v>https://jobs.smartrecruiters.com/wolt/744000020788681</v>
+      </c>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B34" t="str">
+        <v>bolt</v>
+      </c>
+      <c r="C34" t="str">
+        <v>senior fp&amp;a analyst</v>
+      </c>
+      <c r="D34">
+        <v>0</v>
+      </c>
+      <c r="E34" s="1">
+        <v>45377</v>
+      </c>
+      <c r="F34" s="1">
+        <v>45377</v>
+      </c>
+      <c r="G34" t="str">
+        <v>https://careers.bolt.eu/positions/7283230002</v>
+      </c>
+    </row>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B35" t="str">
+        <v>luminor</v>
+      </c>
+      <c r="C35" t="str">
+        <v>senior ict or data oversight risk officer</v>
+      </c>
+      <c r="D35" t="str">
+        <v>other</v>
+      </c>
+      <c r="E35" s="1">
+        <v>45435</v>
+      </c>
+      <c r="F35" s="1">
+        <v>45540</v>
+      </c>
+      <c r="G35" t="str">
+        <v>https://luminorbank.teamtailor.com/jobs/4522272-senior-ict-or-data-oversight-risk-officer</v>
+      </c>
+    </row>
+    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B36" t="str">
+        <v>luminor</v>
+      </c>
+      <c r="C36" t="str">
+        <v>senior it service manager</v>
+      </c>
+      <c r="D36">
+        <v>0</v>
+      </c>
+      <c r="E36" s="1">
+        <v>45377</v>
+      </c>
+      <c r="F36" s="1">
+        <v>45377</v>
+      </c>
+      <c r="G36" t="str">
+        <v>https://luminorbank.teamtailor.com/jobs/3722297-senior-it-service-manager</v>
+      </c>
+    </row>
+    <row r="37" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B37" t="str">
+        <v>rush street interactive</v>
+      </c>
+      <c r="C37" t="str">
+        <v>senior it support engineer</v>
+      </c>
+      <c r="D37" t="str">
+        <v>other</v>
+      </c>
+      <c r="E37" s="1">
+        <v>45583</v>
+      </c>
+      <c r="F37" s="1">
+        <v>45600</v>
+      </c>
+      <c r="G37" t="str">
+        <v>https://job-boards.greenhouse.io/rushstreetinteractive/jobs/5358160004</v>
+      </c>
+    </row>
+    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B38" t="str">
+        <v>seb</v>
+      </c>
+      <c r="C38" t="str">
+        <v>senior linux engineer | seb, tallinn</v>
+      </c>
+      <c r="D38" t="str">
+        <v>other</v>
+      </c>
+      <c r="E38" s="1">
+        <v>45587</v>
+      </c>
+      <c r="F38" s="1">
+        <v>45606</v>
+      </c>
+      <c r="G38" t="str">
+        <v>https://jobs.eu.lever.co/seb/1fc2a460-8b89-4825-b321-a4da147ba394</v>
+      </c>
+    </row>
+    <row r="39" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B39" t="str">
+        <v>seb</v>
+      </c>
+      <c r="C39" t="str">
+        <v>senior linux engineer | seb, tallinn</v>
+      </c>
+      <c r="D39" t="str">
+        <v>other</v>
+      </c>
+      <c r="E39" s="1">
+        <v>45558</v>
+      </c>
+      <c r="F39" s="1">
+        <v>45578</v>
+      </c>
+      <c r="G39" t="str">
+        <v>https://jobs.eu.lever.co/seb/7eb00b81-f92f-4398-9984-28c77339b855</v>
+      </c>
+    </row>
+    <row r="40" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B40" t="str">
+        <v>starship</v>
+      </c>
+      <c r="C40" t="str">
+        <v>senior manufacturing process engineer</v>
+      </c>
+      <c r="D40" t="str">
+        <v>other</v>
+      </c>
+      <c r="E40" s="1">
+        <v>45557</v>
+      </c>
+      <c r="F40" s="1">
+        <v>45587</v>
+      </c>
+      <c r="G40" t="str">
+        <v>https://starship.teamtailor.com/jobs/4940427-senior-manufacturing-process-engineer</v>
+      </c>
+    </row>
+    <row r="41" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B41" t="str">
+        <v>luminor</v>
+      </c>
+      <c r="C41" t="str">
+        <v>senior operational risk officer</v>
+      </c>
+      <c r="D41" t="str">
+        <v>other</v>
+      </c>
+      <c r="E41" s="1">
+        <v>45387</v>
+      </c>
+      <c r="F41" s="1">
+        <v>45400</v>
+      </c>
+      <c r="G41" t="str">
+        <v>https://luminorbank.teamtailor.com/jobs/3794884-senior-operational-risk-officer</v>
+      </c>
+    </row>
+    <row r="42" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B42" t="str">
+        <v>luminor</v>
+      </c>
+      <c r="C42" t="str">
+        <v>senior operational risk officer</v>
+      </c>
+      <c r="D42" t="str">
+        <v>other</v>
+      </c>
+      <c r="E42" s="1">
+        <v>45497</v>
+      </c>
+      <c r="F42" s="1">
+        <v>45606</v>
+      </c>
+      <c r="G42" t="str">
+        <v>https://luminorbank.teamtailor.com/jobs/4761594-senior-operational-risk-officer</v>
+      </c>
+    </row>
+    <row r="43" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B43" t="str">
+        <v>wise</v>
+      </c>
+      <c r="C43" t="str">
+        <v>senior payroll specialist</v>
+      </c>
+      <c r="D43" t="str">
+        <v>other</v>
+      </c>
+      <c r="E43" s="1">
+        <v>45399</v>
+      </c>
+      <c r="F43" s="1">
+        <v>45431</v>
+      </c>
+      <c r="G43" t="str">
+        <v>https://jobs.smartrecruiters.com/wise/743999980854814</v>
+      </c>
+    </row>
+    <row r="44" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B44" t="str">
+        <v>starship</v>
+      </c>
+      <c r="C44" t="str">
+        <v>senior process engineer</v>
+      </c>
+      <c r="D44" t="str">
+        <v>other</v>
+      </c>
+      <c r="E44" s="1">
+        <v>45542</v>
+      </c>
+      <c r="F44" s="1">
+        <v>45555</v>
+      </c>
+      <c r="G44" t="str">
+        <v>https://starship.teamtailor.com/jobs/4940427-senior-process-engineer</v>
+      </c>
+    </row>
+    <row r="45" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B45" t="str">
+        <v>luminor</v>
+      </c>
+      <c r="C45" t="str">
+        <v>senior regulatory officer</v>
+      </c>
+      <c r="D45" t="str">
+        <v>other</v>
+      </c>
+      <c r="E45" s="1">
+        <v>45496</v>
+      </c>
+      <c r="F45" s="1">
+        <v>45522</v>
+      </c>
+      <c r="G45" t="str">
+        <v>https://luminorbank.teamtailor.com/jobs/4756550-senior-regulatory-officer</v>
+      </c>
+    </row>
+    <row r="46" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B46" t="str">
+        <v>wise</v>
+      </c>
+      <c r="C46" t="str">
+        <v>senior service support specialist</v>
+      </c>
+      <c r="D46" t="str">
+        <v>other</v>
+      </c>
+      <c r="E46" s="1">
+        <v>45418</v>
+      </c>
+      <c r="F46" s="1">
+        <v>45418</v>
+      </c>
+      <c r="G46" t="str">
+        <v>https://jobs.smartrecruiters.com/wise/743999985531113</v>
+      </c>
+    </row>
+    <row r="47" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B47" t="str">
+        <v>wise</v>
+      </c>
+      <c r="C47" t="str">
+        <v>senior service support specialist</v>
+      </c>
+      <c r="D47" t="str">
+        <v>other</v>
+      </c>
+      <c r="E47" s="1">
+        <v>45419</v>
+      </c>
+      <c r="F47" s="1">
+        <v>45433</v>
+      </c>
+      <c r="G47" t="str">
+        <v>https://jobs.smartrecruiters.com/wise/743999985746234</v>
+      </c>
+    </row>
+    <row r="48" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B48" t="str">
+        <v>bolt</v>
+      </c>
+      <c r="C48" t="str">
+        <v>senior software engineer, data platform - insights</v>
+      </c>
+      <c r="D48">
+        <v>0</v>
+      </c>
+      <c r="E48" s="1">
+        <v>45377</v>
+      </c>
+      <c r="F48" s="1">
+        <v>45377</v>
+      </c>
+      <c r="G48" t="str">
+        <v>https://careers.bolt.eu/positions/7087991002</v>
+      </c>
+    </row>
+    <row r="49" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B49" t="str">
+        <v>swedbank</v>
+      </c>
+      <c r="C49" t="str">
+        <v>senior solution architect</v>
+      </c>
+      <c r="D49" t="str">
+        <v>other</v>
+      </c>
+      <c r="E49" s="1">
+        <v>45377</v>
+      </c>
+      <c r="F49" s="1">
+        <v>45412</v>
+      </c>
+      <c r="G49" t="str">
+        <v>https://jobs.swedbank.com/jobs/17852-senior-solution-architect</v>
+      </c>
+    </row>
+    <row r="50" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B50" t="str">
+        <v>bolt</v>
+      </c>
+      <c r="C50" t="str">
+        <v>senior tax associate</v>
+      </c>
+      <c r="D50" t="str">
+        <v>other</v>
+      </c>
+      <c r="E50" s="1">
+        <v>45430</v>
+      </c>
+      <c r="F50" s="1">
+        <v>45464</v>
+      </c>
+      <c r="G50" t="str">
+        <v>https://careers.bolt.eu/positions/7452198002</v>
+      </c>
+    </row>
+    <row r="51" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B51" t="str">
+        <v>bolt</v>
+      </c>
+      <c r="C51" t="str">
+        <v>senior tax associate</v>
+      </c>
+      <c r="D51" t="str">
+        <v>other</v>
+      </c>
+      <c r="E51" s="1">
+        <v>45432</v>
+      </c>
+      <c r="F51" s="1">
+        <v>45467</v>
+      </c>
+      <c r="G51" t="str">
+        <v>https://careers.bolt.eu/positions/7454436002</v>
+      </c>
+    </row>
+    <row r="52" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B52" t="str">
+        <v>bolt</v>
+      </c>
+      <c r="C52" t="str">
+        <v>senior tax associate</v>
+      </c>
+      <c r="D52" t="str">
+        <v>other</v>
+      </c>
+      <c r="E52" s="1">
+        <v>45433</v>
+      </c>
+      <c r="F52" s="1">
+        <v>45433</v>
+      </c>
+      <c r="G52" t="str">
+        <v>https://careers.bolt.eu/positions/7454439002</v>
+      </c>
+    </row>
+    <row r="53" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B53" t="str">
+        <v>glia</v>
+      </c>
+      <c r="C53" t="str">
+        <v>senior technical support engineer</v>
+      </c>
+      <c r="D53" t="str">
+        <v>other</v>
+      </c>
+      <c r="E53" s="1">
+        <v>45546</v>
+      </c>
+      <c r="F53" s="1">
+        <v>45587</v>
+      </c>
+      <c r="G53" t="str">
+        <v>https://www.glia.com/jobs/5316733004?gh_jid=5316733004</v>
+      </c>
+    </row>
+    <row r="54" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B54" t="str">
+        <v>wise</v>
+      </c>
+      <c r="C54" t="str">
+        <v>senior technical support technician</v>
+      </c>
+      <c r="D54" t="str">
+        <v>other</v>
+      </c>
+      <c r="E54" s="1">
+        <v>45600</v>
+      </c>
+      <c r="F54" s="1">
+        <v>45606</v>
+      </c>
+      <c r="G54" t="str">
+        <v>https://jobs.smartrecruiters.com/wise/744000024469686</v>
+      </c>
+    </row>
+    <row r="55" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B55" t="str">
+        <v>wise</v>
+      </c>
+      <c r="C55" t="str">
+        <v>senior tooling excellence specialist</v>
+      </c>
+      <c r="D55" t="str">
+        <v>other</v>
+      </c>
+      <c r="E55" s="1">
+        <v>45476</v>
+      </c>
+      <c r="F55" s="1">
+        <v>45479</v>
+      </c>
+      <c r="G55" t="str">
+        <v>https://jobs.smartrecruiters.com/wise/743999998145725</v>
+      </c>
+    </row>
+    <row r="56" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B56" t="str">
+        <v>multitude</v>
+      </c>
+      <c r="C56" t="str">
+        <v>senior underwriter</v>
+      </c>
+      <c r="D56" t="str">
+        <v>other</v>
+      </c>
+      <c r="E56" s="1">
+        <v>45547</v>
+      </c>
+      <c r="F56" s="1">
+        <v>45581</v>
+      </c>
+      <c r="G56" t="str">
+        <v>https://multitude.bamboohr.com/careers/1313</v>
+      </c>
+    </row>
+    <row r="57" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B57" t="str">
+        <v>pipedrive</v>
+      </c>
+      <c r="C57" t="str">
+        <v>senior ux researcher, mixed methods</v>
+      </c>
+      <c r="D57" t="str">
+        <v>other</v>
+      </c>
+      <c r="E57" s="1">
+        <v>45391</v>
+      </c>
+      <c r="F57" s="1">
+        <v>45417</v>
+      </c>
+      <c r="G57" t="str">
+        <v>https://jobs.lever.co/pipedrive/8d9a397d-5e73-43e4-bd1f-4e37f2084934</v>
+      </c>
+    </row>
+    <row r="58" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B58" t="str">
+        <v>bolt</v>
+      </c>
+      <c r="C58" t="str">
+        <v>senior ux writer</v>
+      </c>
+      <c r="D58" t="str">
+        <v>other</v>
+      </c>
+      <c r="E58" s="1">
+        <v>45377</v>
+      </c>
+      <c r="F58" s="1">
+        <v>45450</v>
+      </c>
+      <c r="G58" t="str">
+        <v>https://careers.bolt.eu/positions/7159483002</v>
+      </c>
+    </row>
+    <row r="59" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B59" t="str">
+        <v>bolt</v>
+      </c>
+      <c r="C59" t="str">
+        <v>senior/staff ux researcher, ridehailing</v>
+      </c>
+      <c r="D59" t="str">
+        <v>other</v>
+      </c>
+      <c r="E59" s="1">
+        <v>45388</v>
+      </c>
+      <c r="F59" s="1">
+        <v>45579</v>
+      </c>
+      <c r="G59" t="str">
+        <v>https://careers.bolt.eu/positions/7314800002</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>